<commit_message>
Finished implementing unit removal!  Adjusted the Project_Summary_Template workbook and Help sheet in the WaveAnalyzeTextFiles workbook accordingly
</commit_message>
<xml_diff>
--- a/Excel_Macros/Project_Summary_Template.xlsx
+++ b/Excel_Macros/Project_Summary_Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan_Programming\Programs\WaveAnalysisScripts\Excel_Macros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Danware\Git_Repos\WaveAnalysisScripts\Excel_Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Duration</t>
   </si>
@@ -91,15 +91,6 @@
   </si>
   <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>after</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>Delete?</t>
@@ -194,10 +185,7 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -215,15 +203,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -376,7 +355,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Populations" displayName="Populations" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Populations" displayName="Populations" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Population ID"/>
@@ -389,62 +368,51 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tissues" displayName="Tissues" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tissues" displayName="Tissues" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
-    <tableColumn id="11" name="ID" dataDxfId="27"/>
-    <tableColumn id="9" name="Name" dataDxfId="26"/>
-    <tableColumn id="1" name="Date Prepared" dataDxfId="25"/>
-    <tableColumn id="4" name="Age" dataDxfId="24"/>
-    <tableColumn id="3" name="Sex" dataDxfId="23"/>
-    <tableColumn id="6" name="Genotype" dataDxfId="22"/>
-    <tableColumn id="7" name="Comments" dataDxfId="21"/>
+    <tableColumn id="11" name="ID" dataDxfId="23"/>
+    <tableColumn id="9" name="Name" dataDxfId="22"/>
+    <tableColumn id="1" name="Date Prepared" dataDxfId="21"/>
+    <tableColumn id="4" name="Age" dataDxfId="20"/>
+    <tableColumn id="3" name="Sex" dataDxfId="19"/>
+    <tableColumn id="6" name="Genotype" dataDxfId="18"/>
+    <tableColumn id="7" name="Comments" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Recordings" displayName="Recordings" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Recordings" displayName="Recordings" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:I2"/>
   <tableColumns count="9">
-    <tableColumn id="13" name="ID" dataDxfId="18"/>
-    <tableColumn id="9" name="Tissue ID" dataDxfId="17"/>
-    <tableColumn id="2" name="Recording Number" dataDxfId="16"/>
-    <tableColumn id="10" name="MEA" dataDxfId="15"/>
-    <tableColumn id="5" name="Conditions" dataDxfId="14"/>
-    <tableColumn id="8" name="StartStamp" dataDxfId="13">
+    <tableColumn id="13" name="ID" dataDxfId="14"/>
+    <tableColumn id="9" name="Tissue ID" dataDxfId="13"/>
+    <tableColumn id="2" name="Recording Number" dataDxfId="12"/>
+    <tableColumn id="10" name="MEA" dataDxfId="11"/>
+    <tableColumn id="5" name="Conditions" dataDxfId="10"/>
+    <tableColumn id="8" name="StartStamp" dataDxfId="9">
       <calculatedColumnFormula>IF(Recordings[[#This Row],[Tissue ID]]&lt;&gt;OFFSET(Recordings[[#This Row],[Tissue ID]],-1,0),0,OFFSET(Recordings[[#This Row],[EndStamp]],-1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="EndStamp" dataDxfId="12">
+    <tableColumn id="12" name="EndStamp" dataDxfId="8">
       <calculatedColumnFormula>Recordings[[#This Row],[StartStamp]]+Recordings[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Duration" dataDxfId="11"/>
-    <tableColumn id="14" name="Comments" dataDxfId="10"/>
+    <tableColumn id="3" name="Duration" dataDxfId="7"/>
+    <tableColumn id="14" name="Comments" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Unit_Removal" displayName="Unit_Removal" ref="A6:E7" insertRow="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A6:E7"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Population ID" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Unit_Removal" displayName="Unit_Removal" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D2"/>
+  <tableColumns count="4">
     <tableColumn id="2" name="Tissue ID" dataDxfId="3"/>
     <tableColumn id="3" name="Unit" dataDxfId="2"/>
     <tableColumn id="4" name="Delete?" dataDxfId="1"/>
     <tableColumn id="5" name="Exclude?" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="RemovalTypes" displayName="RemovalTypes" ref="A1:A3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:A3"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Type" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -526,6 +494,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -561,6 +546,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -885,79 +887,57 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D7"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C2"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NexScripts now use Surprise algorithm by default
</commit_message>
<xml_diff>
--- a/Excel_Macros/Project_Summary_Template.xlsx
+++ b/Excel_Macros/Project_Summary_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Populations" sheetId="19" r:id="rId1"/>
@@ -193,15 +193,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -209,17 +209,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -234,15 +234,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -250,18 +261,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -274,19 +277,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -367,27 +367,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Populations" displayName="Populations" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="30" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Populations" displayName="Populations" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Population ID" dataDxfId="29"/>
     <tableColumn id="4" name="Name" dataDxfId="28"/>
-    <tableColumn id="3" name="Abbreviation" dataDxfId="26"/>
-    <tableColumn id="2" name="Control?" dataDxfId="27"/>
+    <tableColumn id="3" name="Abbreviation" dataDxfId="27"/>
+    <tableColumn id="2" name="Control?" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tissues" displayName="Tissues" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tissues" displayName="Tissues" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
-    <tableColumn id="11" name="ID" dataDxfId="21"/>
-    <tableColumn id="9" name="Name" dataDxfId="19"/>
-    <tableColumn id="1" name="Date Prepared" dataDxfId="20"/>
-    <tableColumn id="4" name="Age" dataDxfId="23"/>
-    <tableColumn id="3" name="Sex" dataDxfId="22"/>
+    <tableColumn id="11" name="ID" dataDxfId="23"/>
+    <tableColumn id="9" name="Name" dataDxfId="22"/>
+    <tableColumn id="1" name="Date Prepared" dataDxfId="21"/>
+    <tableColumn id="4" name="Age" dataDxfId="20"/>
+    <tableColumn id="3" name="Sex" dataDxfId="19"/>
     <tableColumn id="6" name="Genotype" dataDxfId="18"/>
     <tableColumn id="7" name="Comments" dataDxfId="17"/>
   </tableColumns>
@@ -396,18 +396,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Recordings" displayName="Recordings" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Recordings" displayName="Recordings" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:I2"/>
   <tableColumns count="9">
     <tableColumn id="13" name="ID" dataDxfId="14"/>
     <tableColumn id="9" name="Tissue ID" dataDxfId="13"/>
     <tableColumn id="2" name="Recording Number" dataDxfId="12"/>
-    <tableColumn id="10" name="MEA" dataDxfId="10"/>
-    <tableColumn id="5" name="Conditions" dataDxfId="8"/>
+    <tableColumn id="10" name="MEA" dataDxfId="11"/>
+    <tableColumn id="5" name="Conditions" dataDxfId="10"/>
     <tableColumn id="8" name="StartStamp" dataDxfId="9">
       <calculatedColumnFormula>IF(Recordings[[#This Row],[Tissue ID]]&lt;&gt;OFFSET(Recordings[[#This Row],[Tissue ID]],-1,0),0,OFFSET(Recordings[[#This Row],[EndStamp]],-1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="EndStamp" dataDxfId="11">
+    <tableColumn id="12" name="EndStamp" dataDxfId="8">
       <calculatedColumnFormula>Recordings[[#This Row],[StartStamp]]+Recordings[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Duration" dataDxfId="7"/>
@@ -418,13 +418,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Unit_Removal" displayName="Unit_Removal" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Unit_Removal" displayName="Unit_Removal" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
-    <tableColumn id="2" name="Tissue ID" dataDxfId="2"/>
-    <tableColumn id="3" name="Unit" dataDxfId="0"/>
+    <tableColumn id="2" name="Tissue ID" dataDxfId="3"/>
+    <tableColumn id="3" name="Unit" dataDxfId="2"/>
     <tableColumn id="4" name="Delete?" dataDxfId="1"/>
-    <tableColumn id="5" name="Exclude?" dataDxfId="5"/>
+    <tableColumn id="5" name="Exclude?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,7 +696,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +870,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>